<commit_message>
Begin working on Excel local data upload
</commit_message>
<xml_diff>
--- a/stock_score_data.xlsx
+++ b/stock_score_data.xlsx
@@ -1,33 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacklm/Documents/stockScore/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" tabRatio="500"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="14420" windowWidth="25600" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" concurrentCalc="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
   <si>
     <t>Last updated</t>
   </si>
@@ -35,22 +22,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,22 +53,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -347,28 +328,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="12.1640625"/>
+    <col customWidth="1" max="2" min="2" width="19.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>43268.948645833319</v>
+      <c r="B1" s="1" t="n">
+        <v>43268.94864583332</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>